<commit_message>
Implemented Spot light and Point light
</commit_message>
<xml_diff>
--- a/Alwin_Hill_DevIVProjectRubric.xlsx
+++ b/Alwin_Hill_DevIVProjectRubric.xlsx
@@ -77,7 +77,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="81">
   <si>
     <t>Apply a post process routine via pixel shader (eg Blur or Custom Pixel Maipulations)</t>
   </si>
@@ -969,8 +969,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L117"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F33" sqref="F33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1102,7 +1102,7 @@
       </c>
       <c r="I4" s="18">
         <f>IF(SUMIF(E4:E85,"=II",G4:G85) + SUMIF(D90:D91, "X",B90:B91) &gt; 18, 18, SUMIF(E4:E85,"=II",G4:G85) + SUMIF(D90:D91, "X",B90:B91))</f>
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="J4" s="18">
         <f>IF(SUMIF(E4:E85,"=III",G4:G85) + SUMIF(E90:E91, "X",B90:B91) &gt; 18, 18, SUMIF(E4:E85,"=III",G4:G85) + SUMIF(E90:E91, "X",B90:B91))</f>
@@ -1114,7 +1114,7 @@
       </c>
       <c r="L4" s="18">
         <f>SUM(G4:G85) + SUMIF(C90:C91, "X",B90:B91) + SUMIF(D90:D91, "X",B90:B91) + SUMIF(E90:E91, "X",B90:B91)</f>
-        <v>20</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -1251,7 +1251,7 @@
       </c>
       <c r="I8" s="18">
         <f>I4+IF(I4 &lt; 18, IF(H10+I4 &gt; 18, 18- I4, H10),0)</f>
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="J8" s="18">
         <f>J4+IF(J4 &lt; 18, IF(I10+J4 &gt; 18, 18- J4, I10),0)</f>
@@ -1742,10 +1742,12 @@
       <c r="E30" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="F30" s="3"/>
+      <c r="F30" s="3" t="s">
+        <v>78</v>
+      </c>
       <c r="G30" s="17">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H30" s="5"/>
       <c r="I30" s="5"/>
@@ -1766,11 +1768,15 @@
       <c r="D31" s="5">
         <v>2</v>
       </c>
-      <c r="E31" s="2"/>
-      <c r="F31" s="3"/>
+      <c r="E31" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="F31" s="3" t="s">
+        <v>78</v>
+      </c>
       <c r="G31" s="17">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H31" s="5"/>
       <c r="I31" s="5"/>
@@ -1791,11 +1797,15 @@
       <c r="D32" s="5">
         <v>2</v>
       </c>
-      <c r="E32" s="2"/>
-      <c r="F32" s="3"/>
+      <c r="E32" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="F32" s="3" t="s">
+        <v>78</v>
+      </c>
       <c r="G32" s="17">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H32" s="5"/>
       <c r="I32" s="5"/>
@@ -1816,11 +1826,15 @@
       <c r="D33" s="5">
         <v>1</v>
       </c>
-      <c r="E33" s="2"/>
-      <c r="F33" s="3"/>
+      <c r="E33" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="F33" s="3" t="s">
+        <v>78</v>
+      </c>
       <c r="G33" s="17">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H33" s="5"/>
       <c r="I33" s="5"/>
@@ -1841,11 +1855,15 @@
       <c r="D34" s="5">
         <v>1</v>
       </c>
-      <c r="E34" s="2"/>
-      <c r="F34" s="3"/>
+      <c r="E34" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="F34" s="3" t="s">
+        <v>78</v>
+      </c>
       <c r="G34" s="17">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H34" s="5"/>
       <c r="I34" s="5"/>
@@ -3106,7 +3124,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L6 K4 H6:J6">
+  <conditionalFormatting sqref="K4 L6 H6:J6">
     <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="num" val="0"/>

</xml_diff>

<commit_message>
Made some changes to normal mapping and added barrel model to show normal mapping
</commit_message>
<xml_diff>
--- a/Alwin_Hill_DevIVProjectRubric.xlsx
+++ b/Alwin_Hill_DevIVProjectRubric.xlsx
@@ -77,7 +77,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="82">
   <si>
     <t>Apply a post process routine via pixel shader (eg Blur or Custom Pixel Maipulations)</t>
   </si>
@@ -372,6 +372,9 @@
   </si>
   <si>
     <t>II</t>
+  </si>
+  <si>
+    <t>III</t>
   </si>
 </sst>
 </file>
@@ -969,8 +972,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L117"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F39" sqref="F39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1106,15 +1109,15 @@
       </c>
       <c r="J4" s="18">
         <f>IF(SUMIF(E4:E85,"=III",G4:G85) + SUMIF(E90:E91, "X",B90:B91) &gt; 18, 18, SUMIF(E4:E85,"=III",G4:G85) + SUMIF(E90:E91, "X",B90:B91))</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="K4" s="18">
         <f>SUM(H6,I6,J6)</f>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="L4" s="18">
         <f>SUM(G4:G85) + SUMIF(C90:C91, "X",B90:B91) + SUMIF(D90:D91, "X",B90:B91) + SUMIF(E90:E91, "X",B90:B91)</f>
-        <v>37</v>
+        <v>46</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -1183,7 +1186,7 @@
       </c>
       <c r="I6" s="18">
         <f>IF(SUMIF(E4:E85,"=II",G4:G85) + SUMIF(D90:D91, "X",B90:B91) &gt; 18, SUMIF(E4:E85,"=II",G4:G85) + SUMIF(D90:D91, "X",B90:B91) - 18,0)</f>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="J6" s="18">
         <f>IF(SUMIF(E4:E85,"=III",G4:G85) + SUMIF(E90:E91, "X",B90:B91) &gt; 18, SUMIF(E4:E85,"=III",G4:G85) + SUMIF(E90:E91, "X",B90:B91) - 18,0)</f>
@@ -1255,7 +1258,7 @@
       </c>
       <c r="J8" s="18">
         <f>J4+IF(J4 &lt; 18, IF(I10+J4 &gt; 18, 18- J4, I10),0)</f>
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="K8" s="5"/>
       <c r="L8" s="5"/>
@@ -1304,23 +1307,19 @@
       <c r="D10" s="5">
         <v>1</v>
       </c>
-      <c r="E10" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="F10" s="3" t="s">
-        <v>78</v>
-      </c>
+      <c r="E10" s="2"/>
+      <c r="F10" s="3"/>
       <c r="G10" s="17">
         <f xml:space="preserve"> IF(EXACT(F10,"X"),IF(EXACT(E10,"I"),$B10,IF(EXACT(E10,"II"),$C10,IF(EXACT(E10,"III"),$D10,0))),0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H10" s="20">
         <f>IF(K4+H4 - 18 &gt; 0, K4+H4 - 18, 0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I10" s="20">
         <f>IF(H10+I4 - 18 &gt; 0, H10+I4 - 18, 0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J10" s="20">
         <f>IF(I10+J4 - 18 &gt; 0, I10+J4 - 18, 0)</f>
@@ -1577,11 +1576,15 @@
       <c r="D22" s="5">
         <v>2</v>
       </c>
-      <c r="E22" s="2"/>
-      <c r="F22" s="3"/>
+      <c r="E22" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="F22" s="3" t="s">
+        <v>78</v>
+      </c>
       <c r="G22" s="17">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H22" s="5"/>
       <c r="I22" s="5"/>
@@ -2574,11 +2577,15 @@
       <c r="D67" s="5">
         <v>4</v>
       </c>
-      <c r="E67" s="2"/>
-      <c r="F67" s="3"/>
+      <c r="E67" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="F67" s="3" t="s">
+        <v>78</v>
+      </c>
       <c r="G67" s="17">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H67" s="5"/>
       <c r="I67" s="5"/>
@@ -2599,11 +2606,15 @@
       <c r="D68" s="5">
         <v>4</v>
       </c>
-      <c r="E68" s="2"/>
-      <c r="F68" s="3"/>
+      <c r="E68" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="F68" s="3" t="s">
+        <v>78</v>
+      </c>
       <c r="G68" s="17">
         <f t="shared" ref="G68:G85" si="2" xml:space="preserve"> IF(EXACT(F68,"X"),IF(EXACT(E68,"I"),$B68,IF(EXACT(E68,"II"),$C68,IF(EXACT(E68,"III"),$D68,0))),0)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H68" s="5"/>
       <c r="I68" s="5"/>
@@ -3136,7 +3147,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K4 L6 H6:J6">
+  <conditionalFormatting sqref="L6 K4 H6:J6">
     <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="num" val="0"/>

</xml_diff>